<commit_message>
fix  the tenant and boundary and dropdwon issue
</commit_message>
<xml_diff>
--- a/utilities/crs_dataloader/templates/Common and Complaint Master.xlsx
+++ b/utilities/crs_dataloader/templates/Common and Complaint Master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salaudeenn/Documents/urban/CCRS/ccrs/Citizen-Complaint-Resolution-System/utilities/pgr_dataLoader/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salaudeenn/Documents/urban/CCRS/ccrs/test/Citizen-Complaint-Resolution-System/utilities/crs_dataloader/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5462174E-AE6E-E44C-9E73-248521BB5161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81109A8-3CA6-B944-BB77-F902E6906222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="15480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="117">
   <si>
     <t>COMMON MASTER TEMPLATE - USER GUIDE</t>
   </si>
@@ -364,15 +364,6 @@
   </si>
   <si>
     <t>water tab,water supply</t>
-  </si>
-  <si>
-    <t>WATER not coming</t>
-  </si>
-  <si>
-    <t>RAV</t>
-  </si>
-  <si>
-    <t>CAR</t>
   </si>
   <si>
     <t xml:space="preserve">Water Supply | No Water | WATER DEPARTMENT | 24 | water,no supply,dry tap | </t>
@@ -726,7 +717,7 @@
   </sheetPr>
   <dimension ref="A1:A152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1305,17 +1296,17 @@
     </row>
     <row r="129" spans="1:1" ht="15" x14ac:dyDescent="0.15">
       <c r="A129" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15" x14ac:dyDescent="0.15">
       <c r="A130" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15" x14ac:dyDescent="0.15">
       <c r="A131" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="13" x14ac:dyDescent="0.15">
@@ -1419,7 +1410,9 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5456,7 +5449,9 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5503,21 +5498,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>105</v>
-      </c>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="7" t="s">
-        <v>116</v>
-      </c>
+      <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="E4" s="7"/>
     </row>

</xml_diff>